<commit_message>
Day 1, exercise 4
</commit_message>
<xml_diff>
--- a/Ex ET11 - Lizard data.xlsx
+++ b/Ex ET11 - Lizard data.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="54">
   <si>
     <t>Sinervo's data (1990-1999):</t>
   </si>
@@ -200,10 +200,10 @@
     <t>Normalized</t>
   </si>
   <si>
-    <t>Mono</t>
+    <t>Females monopolized</t>
   </si>
   <si>
-    <t>Shared</t>
+    <t>Females shared</t>
   </si>
   <si>
     <t>Year</t>
@@ -1441,7 +1441,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Normal 2" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Normal 2" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1506,7 +1506,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1900,6 +1900,28 @@
           </c:marker>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="99ccff"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:hiLowLines>
           <c:spPr>
             <a:ln>
@@ -1913,11 +1935,11 @@
           <c:downBars/>
         </c:upDownBars>
         <c:marker val="1"/>
-        <c:axId val="73331803"/>
-        <c:axId val="93308345"/>
+        <c:axId val="44159988"/>
+        <c:axId val="29215333"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="73331803"/>
+        <c:axId val="44159988"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1953,14 +1975,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="93308345"/>
+        <c:crossAx val="29215333"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93308345"/>
+        <c:axId val="29215333"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2005,7 +2027,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="73331803"/>
+        <c:crossAx val="44159988"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2030,7 +2052,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2399,8 +2421,8 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="95541368"/>
-        <c:axId val="50500479"/>
+        <c:axId val="96025352"/>
+        <c:axId val="8145214"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -5825,11 +5847,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="69486857"/>
-        <c:axId val="68686274"/>
+        <c:axId val="91093740"/>
+        <c:axId val="79005709"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95541368"/>
+        <c:axId val="96025352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.1"/>
@@ -5848,11 +5870,11 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="50500479"/>
+        <c:crossAx val="8145214"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="50500479"/>
+        <c:axId val="8145214"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.05"/>
@@ -5871,11 +5893,11 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="95541368"/>
+        <c:crossAx val="96025352"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69486857"/>
+        <c:axId val="91093740"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.1"/>
@@ -5894,11 +5916,11 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="68686274"/>
+        <c:crossAx val="79005709"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="68686274"/>
+        <c:axId val="79005709"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.05"/>
@@ -5917,7 +5939,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="69486857"/>
+        <c:crossAx val="91093740"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -5948,15 +5970,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>90720</xdr:colOff>
+      <xdr:colOff>117720</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>185040</xdr:rowOff>
+      <xdr:rowOff>176040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>79920</xdr:colOff>
+      <xdr:colOff>106560</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>28800</xdr:rowOff>
+      <xdr:rowOff>19440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5969,8 +5991,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3961440" y="387360"/>
-          <a:ext cx="3215160" cy="2679840"/>
+          <a:off x="3988440" y="378360"/>
+          <a:ext cx="3214800" cy="2679480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5985,15 +6007,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>81360</xdr:colOff>
+      <xdr:colOff>108360</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>167040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>34920</xdr:colOff>
+      <xdr:colOff>61560</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>29520</xdr:rowOff>
+      <xdr:rowOff>20160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6006,8 +6028,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3952080" y="4024440"/>
-          <a:ext cx="3179520" cy="3702240"/>
+          <a:off x="3979080" y="4015440"/>
+          <a:ext cx="3179160" cy="3701880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6022,15 +6044,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>434520</xdr:colOff>
+      <xdr:colOff>461520</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>116280</xdr:rowOff>
+      <xdr:rowOff>107280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>387000</xdr:colOff>
+      <xdr:colOff>413640</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:rowOff>104760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6038,8 +6060,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4305240" y="3154680"/>
-        <a:ext cx="5758920" cy="3238920"/>
+        <a:off x="4332240" y="3145680"/>
+        <a:ext cx="5758560" cy="3238560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6057,15 +6079,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>64080</xdr:colOff>
+      <xdr:colOff>91080</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>163440</xdr:rowOff>
+      <xdr:rowOff>154440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>43920</xdr:colOff>
+      <xdr:colOff>70560</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>187200</xdr:rowOff>
+      <xdr:rowOff>177840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6073,8 +6095,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5141520" y="163440"/>
-        <a:ext cx="5725080" cy="4847040"/>
+        <a:off x="5168520" y="154440"/>
+        <a:ext cx="5724720" cy="4846680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6095,7 +6117,7 @@
   <dimension ref="B1:AE508"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U8" activeCellId="0" sqref="U8"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95"/>
@@ -50151,38 +50173,39 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N12" activeCellId="0" sqref="N12"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="10" min="1" style="0" width="5.13775510204082"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="5.69897959183674"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="5.13775510204082"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>49</v>
       </c>
       <c r="H1" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="0" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="K2" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="N2" s="0" t="s">
         <v>52</v>
       </c>
     </row>
@@ -50226,51 +50249,69 @@
       <c r="M3" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="N3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>1991</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
+        <v>0.126</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0.124</v>
+      </c>
+      <c r="E4" s="0" t="n">
         <v>0.3</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="F4" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="G4" s="0" t="n">
         <v>2.2</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="H4" s="0" t="n">
         <v>0.4</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="I4" s="0" t="n">
         <v>0.2</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="J4" s="0" t="n">
         <v>0.3</v>
       </c>
-      <c r="H4" s="0" t="n">
-        <f aca="false">B4/(SUM($B4:$D4))</f>
+      <c r="K4" s="0" t="n">
+        <f aca="false">E4/(SUM($E4:$G4))</f>
         <v>0.1</v>
       </c>
-      <c r="I4" s="0" t="n">
-        <f aca="false">C4/(SUM($B4:$D4))</f>
+      <c r="L4" s="0" t="n">
+        <f aca="false">F4/(SUM($E4:$G4))</f>
         <v>0.166666666666667</v>
       </c>
-      <c r="J4" s="0" t="n">
-        <f aca="false">D4/(SUM($B4:$D4))</f>
+      <c r="M4" s="0" t="n">
+        <f aca="false">G4/(SUM($E4:$G4))</f>
         <v>0.733333333333333</v>
       </c>
-      <c r="K4" s="0" t="n">
-        <f aca="false">E4/SUM($E4:$G4)</f>
+      <c r="N4" s="0" t="n">
+        <f aca="false">H4/SUM($H4:$J4)</f>
         <v>0.444444444444444</v>
       </c>
-      <c r="L4" s="0" t="n">
-        <f aca="false">F4/SUM($E4:$G4)</f>
+      <c r="O4" s="0" t="n">
+        <f aca="false">I4/SUM($H4:$J4)</f>
         <v>0.222222222222222</v>
       </c>
-      <c r="M4" s="0" t="n">
-        <f aca="false">G4/SUM($E4:$G4)</f>
+      <c r="P4" s="0" t="n">
+        <f aca="false">J4/SUM($H4:$J4)</f>
         <v>0.333333333333333</v>
       </c>
     </row>
@@ -50278,46 +50319,55 @@
       <c r="A5" s="0" t="n">
         <v>1992</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
+        <v>0.361</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>0.328</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0.311</v>
+      </c>
+      <c r="E5" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="F5" s="0" t="n">
         <v>0.8</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="G5" s="0" t="n">
         <v>0.8</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="H5" s="0" t="n">
         <v>0.2</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="I5" s="0" t="n">
         <v>0.3</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="J5" s="0" t="n">
         <v>0.3</v>
       </c>
-      <c r="H5" s="0" t="n">
-        <f aca="false">B5/(SUM($B5:$D5))</f>
+      <c r="K5" s="0" t="n">
+        <f aca="false">E5/(SUM($E5:$G5))</f>
         <v>0.238095238095238</v>
       </c>
-      <c r="I5" s="0" t="n">
-        <f aca="false">C5/(SUM($B5:$D5))</f>
+      <c r="L5" s="0" t="n">
+        <f aca="false">F5/(SUM($E5:$G5))</f>
         <v>0.380952380952381</v>
       </c>
-      <c r="J5" s="0" t="n">
-        <f aca="false">D5/(SUM($B5:$D5))</f>
+      <c r="M5" s="0" t="n">
+        <f aca="false">G5/(SUM($E5:$G5))</f>
         <v>0.380952380952381</v>
       </c>
-      <c r="K5" s="0" t="n">
-        <f aca="false">E5/SUM($E5:$G5)</f>
+      <c r="N5" s="0" t="n">
+        <f aca="false">H5/SUM($H5:$J5)</f>
         <v>0.25</v>
       </c>
-      <c r="L5" s="0" t="n">
-        <f aca="false">F5/SUM($E5:$G5)</f>
+      <c r="O5" s="0" t="n">
+        <f aca="false">I5/SUM($H5:$J5)</f>
         <v>0.375</v>
       </c>
-      <c r="M5" s="0" t="n">
-        <f aca="false">G5/SUM($E5:$G5)</f>
+      <c r="P5" s="0" t="n">
+        <f aca="false">J5/SUM($H5:$J5)</f>
         <v>0.375</v>
       </c>
     </row>
@@ -50325,46 +50375,55 @@
       <c r="A6" s="0" t="n">
         <v>1993</v>
       </c>
-      <c r="B6" s="0" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>0.35</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>0.45</v>
+      <c r="B6" s="1" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>0.321</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>0.259</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>0.45</v>
       </c>
       <c r="F6" s="0" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I6" s="0" t="n">
         <v>0.25</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="J6" s="0" t="n">
         <v>0.3</v>
       </c>
-      <c r="H6" s="0" t="n">
-        <f aca="false">B6/(SUM($B6:$D6))</f>
+      <c r="K6" s="0" t="n">
+        <f aca="false">E6/(SUM($E6:$G6))</f>
         <v>0.36</v>
       </c>
-      <c r="I6" s="0" t="n">
-        <f aca="false">C6/(SUM($B6:$D6))</f>
+      <c r="L6" s="0" t="n">
+        <f aca="false">F6/(SUM($E6:$G6))</f>
         <v>0.28</v>
       </c>
-      <c r="J6" s="0" t="n">
-        <f aca="false">D6/(SUM($B6:$D6))</f>
+      <c r="M6" s="0" t="n">
+        <f aca="false">G6/(SUM($E6:$G6))</f>
         <v>0.36</v>
       </c>
-      <c r="K6" s="0" t="n">
-        <f aca="false">E6/SUM($E6:$G6)</f>
+      <c r="N6" s="0" t="n">
+        <f aca="false">H6/SUM($H6:$J6)</f>
         <v>0.45</v>
       </c>
-      <c r="L6" s="0" t="n">
-        <f aca="false">F6/SUM($E6:$G6)</f>
+      <c r="O6" s="0" t="n">
+        <f aca="false">I6/SUM($H6:$J6)</f>
         <v>0.25</v>
       </c>
-      <c r="M6" s="0" t="n">
-        <f aca="false">G6/SUM($E6:$G6)</f>
+      <c r="P6" s="0" t="n">
+        <f aca="false">J6/SUM($H6:$J6)</f>
         <v>0.3</v>
       </c>
     </row>
@@ -50372,46 +50431,55 @@
       <c r="A7" s="0" t="n">
         <v>1994</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
+        <v>0.485</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>0.389</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>0.126</v>
+      </c>
+      <c r="E7" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="F7" s="0" t="n">
         <v>0.35</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="G7" s="0" t="n">
         <v>0.55</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="H7" s="0" t="n">
         <v>0.8</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="I7" s="0" t="n">
         <v>0.6</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="J7" s="0" t="n">
         <v>0.8</v>
       </c>
-      <c r="H7" s="0" t="n">
-        <f aca="false">B7/(SUM($B7:$D7))</f>
+      <c r="K7" s="0" t="n">
+        <f aca="false">E7/(SUM($E7:$G7))</f>
         <v>0.1</v>
       </c>
-      <c r="I7" s="0" t="n">
-        <f aca="false">C7/(SUM($B7:$D7))</f>
+      <c r="L7" s="0" t="n">
+        <f aca="false">F7/(SUM($E7:$G7))</f>
         <v>0.35</v>
       </c>
-      <c r="J7" s="0" t="n">
-        <f aca="false">D7/(SUM($B7:$D7))</f>
+      <c r="M7" s="0" t="n">
+        <f aca="false">G7/(SUM($E7:$G7))</f>
         <v>0.55</v>
       </c>
-      <c r="K7" s="0" t="n">
-        <f aca="false">E7/SUM($E7:$G7)</f>
+      <c r="N7" s="0" t="n">
+        <f aca="false">H7/SUM($H7:$J7)</f>
         <v>0.363636363636364</v>
       </c>
-      <c r="L7" s="0" t="n">
-        <f aca="false">F7/SUM($E7:$G7)</f>
+      <c r="O7" s="0" t="n">
+        <f aca="false">I7/SUM($H7:$J7)</f>
         <v>0.272727272727273</v>
       </c>
-      <c r="M7" s="0" t="n">
-        <f aca="false">G7/SUM($E7:$G7)</f>
+      <c r="P7" s="0" t="n">
+        <f aca="false">J7/SUM($H7:$J7)</f>
         <v>0.363636363636364</v>
       </c>
     </row>
@@ -50419,72 +50487,81 @@
       <c r="A8" s="0" t="n">
         <v>1995</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>0.551</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>0.099</v>
+      </c>
+      <c r="E8" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="F8" s="0" t="n">
         <v>0.05</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>0.6</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H8" s="0" t="n">
-        <f aca="false">B8/(SUM($B8:$D8))</f>
+        <v>0.65</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <f aca="false">E8/(SUM($E8:$G8))</f>
         <v>0.0869565217391305</v>
       </c>
-      <c r="I8" s="0" t="n">
-        <f aca="false">C8/(SUM($B8:$D8))</f>
+      <c r="L8" s="0" t="n">
+        <f aca="false">F8/(SUM($E8:$G8))</f>
         <v>0.0434782608695652</v>
       </c>
-      <c r="J8" s="0" t="n">
-        <f aca="false">D8/(SUM($B8:$D8))</f>
+      <c r="M8" s="0" t="n">
+        <f aca="false">G8/(SUM($E8:$G8))</f>
         <v>0.869565217391304</v>
       </c>
-      <c r="K8" s="0" t="n">
-        <f aca="false">E8/SUM($E8:$G8)</f>
+      <c r="N8" s="0" t="n">
+        <f aca="false">H8/SUM($H8:$J8)</f>
         <v>0.288888888888889</v>
       </c>
-      <c r="L8" s="0" t="n">
-        <f aca="false">F8/SUM($E8:$G8)</f>
+      <c r="O8" s="0" t="n">
+        <f aca="false">I8/SUM($H8:$J8)</f>
         <v>0.266666666666667</v>
       </c>
-      <c r="M8" s="0" t="n">
-        <f aca="false">G8/SUM($E8:$G8)</f>
+      <c r="P8" s="0" t="n">
+        <f aca="false">J8/SUM($H8:$J8)</f>
         <v>0.444444444444444</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H10" s="0" t="n">
-        <f aca="false">SUM(H4:H8)/SUM($H$4:$J$8)</f>
+        <f aca="false">SUM(K4:K8)/SUM($K$4:$M$8)</f>
         <v>0.177010351966874</v>
       </c>
       <c r="I10" s="0" t="n">
-        <f aca="false">SUM(I4:I8)/SUM($H$4:$J$8)</f>
+        <f aca="false">SUM(L4:L8)/SUM($K$4:$M$8)</f>
         <v>0.244219461697723</v>
       </c>
       <c r="J10" s="0" t="n">
-        <f aca="false">SUM(J4:J8)/SUM($H$4:$J$8)</f>
+        <f aca="false">SUM(M4:M8)/SUM($K$4:$M$8)</f>
         <v>0.578770186335404</v>
       </c>
       <c r="K10" s="0" t="n">
-        <f aca="false">SUM(K4:K8)/SUM($K$4:$M$8)</f>
+        <f aca="false">SUM(N4:N8)/SUM($N$4:$P$8)</f>
         <v>0.359393939393939</v>
       </c>
       <c r="L10" s="0" t="n">
-        <f aca="false">SUM(L4:L8)/SUM($K$4:$M$8)</f>
+        <f aca="false">SUM(O4:O8)/SUM($N$4:$P$8)</f>
         <v>0.277323232323232</v>
       </c>
       <c r="M10" s="0" t="n">
-        <f aca="false">SUM(M4:M8)/SUM($K$4:$M$8)</f>
+        <f aca="false">SUM(P4:P8)/SUM($N$4:$P$8)</f>
         <v>0.363282828282828</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Also plot predicted values
</commit_message>
<xml_diff>
--- a/Ex ET11 - Lizard data.xlsx
+++ b/Ex ET11 - Lizard data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="937" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="937" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -1441,7 +1441,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Normal 2" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal 2" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1922,6 +1922,28 @@
           </c:marker>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="99ccff"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:hiLowLines>
           <c:spPr>
             <a:ln>
@@ -1935,11 +1957,11 @@
           <c:downBars/>
         </c:upDownBars>
         <c:marker val="1"/>
-        <c:axId val="44159988"/>
-        <c:axId val="29215333"/>
+        <c:axId val="97362879"/>
+        <c:axId val="51937847"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="44159988"/>
+        <c:axId val="97362879"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1975,14 +1997,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="29215333"/>
+        <c:crossAx val="51937847"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="29215333"/>
+        <c:axId val="51937847"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2027,7 +2049,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="44159988"/>
+        <c:crossAx val="97362879"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2421,8 +2443,8 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="96025352"/>
-        <c:axId val="8145214"/>
+        <c:axId val="12353095"/>
+        <c:axId val="54351464"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -5847,11 +5869,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="91093740"/>
-        <c:axId val="79005709"/>
+        <c:axId val="20153406"/>
+        <c:axId val="92797758"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="96025352"/>
+        <c:axId val="12353095"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.1"/>
@@ -5870,11 +5892,11 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="8145214"/>
+        <c:crossAx val="54351464"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="8145214"/>
+        <c:axId val="54351464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.05"/>
@@ -5893,11 +5915,11 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="96025352"/>
+        <c:crossAx val="12353095"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91093740"/>
+        <c:axId val="20153406"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.1"/>
@@ -5916,11 +5938,11 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="79005709"/>
+        <c:crossAx val="92797758"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="79005709"/>
+        <c:axId val="92797758"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.05"/>
@@ -5939,7 +5961,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="91093740"/>
+        <c:crossAx val="20153406"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -5970,15 +5992,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>117720</xdr:colOff>
+      <xdr:colOff>144720</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>167040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>106560</xdr:colOff>
+      <xdr:colOff>133200</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>19440</xdr:rowOff>
+      <xdr:rowOff>10080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5991,8 +6013,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3988440" y="378360"/>
-          <a:ext cx="3214800" cy="2679480"/>
+          <a:off x="4015440" y="369360"/>
+          <a:ext cx="3214440" cy="2679120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6007,15 +6029,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>108360</xdr:colOff>
+      <xdr:colOff>135360</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>167040</xdr:rowOff>
+      <xdr:rowOff>158040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>61560</xdr:colOff>
+      <xdr:colOff>88200</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>20160</xdr:rowOff>
+      <xdr:rowOff>10800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6028,8 +6050,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3979080" y="4015440"/>
-          <a:ext cx="3179160" cy="3701880"/>
+          <a:off x="4006080" y="4006440"/>
+          <a:ext cx="3178800" cy="3701520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6044,15 +6066,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>461520</xdr:colOff>
+      <xdr:colOff>488520</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>107280</xdr:rowOff>
+      <xdr:rowOff>98280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>413640</xdr:colOff>
+      <xdr:colOff>440280</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>104760</xdr:rowOff>
+      <xdr:rowOff>95400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6060,8 +6082,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4332240" y="3145680"/>
-        <a:ext cx="5758560" cy="3238560"/>
+        <a:off x="4359240" y="3136680"/>
+        <a:ext cx="5758200" cy="3238200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6079,15 +6101,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>91080</xdr:colOff>
+      <xdr:colOff>118080</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>154440</xdr:rowOff>
+      <xdr:rowOff>145440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>70560</xdr:colOff>
+      <xdr:colOff>97200</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6095,8 +6117,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5168520" y="154440"/>
-        <a:ext cx="5724720" cy="4846680"/>
+        <a:off x="5195520" y="145440"/>
+        <a:ext cx="5724360" cy="4846320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6116,8 +6138,8 @@
   </sheetPr>
   <dimension ref="B1:AE508"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T8" activeCellId="0" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95"/>
@@ -41702,7 +41724,7 @@
   <dimension ref="A1:AR110"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -50175,11 +50197,14 @@
   </sheetPr>
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E1" s="0" t="s">

</xml_diff>